<commit_message>
XPathHelper utility class for building xpath selector
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/CurrencyTemplate.xlsx
+++ b/src/main/resources/templates/CurrencyTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borda\IdeaProjects\AnanasTraining\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F54475-F274-4801-9D8B-0BB47B2BE394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DA2724-05A2-495F-82A5-E4C649BB632C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Currency</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>JPY</t>
+  </si>
+  <si>
+    <t>TRY</t>
   </si>
 </sst>
 </file>
@@ -111,8 +114,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Currency"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Code"/>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +466,14 @@
         <v>392</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>949</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>